<commit_message>
update data to do poc
</commit_message>
<xml_diff>
--- a/Position.xlsx
+++ b/Position.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRA81HC\Desktop\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RolesStructure\project\orgchart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Principal Consultant</t>
+  </si>
+  <si>
+    <t>Member Engineering</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -412,134 +415,145 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>